<commit_message>
feat: remove empty rows in Excel file
</commit_message>
<xml_diff>
--- a/generate-excel/src/test/resources/e2e/timesheet_PiedPiper_20220101-20221231.xlsx
+++ b/generate-excel/src/test/resources/e2e/timesheet_PiedPiper_20220101-20221231.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tino/IdeaProjects/timesheet-wizard/generate-excel/src/test/resources/e2e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD42C910-B70A-424B-BC26-655B54DE01AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F6DC6B-18BC-8947-86B6-9FCAF31C25AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -247,22 +247,127 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF2C5282"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF2C5282"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF2C5282"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF2C5282"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF2C5282"/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -271,138 +376,20 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF2C5282"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF2C5282"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color rgb="FF2C5282"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF2C5282"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF2C5282"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF2C5282"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF2C5282"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF2C5282"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF2C5282"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF2C5282"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF2C5282"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF2C5282"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF2C5282"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF2C5282"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF2C5282"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF2C5282"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF2C5282"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF2C5282"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF2C5282"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF2C5282"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -442,80 +429,86 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="8" applyFont="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="10" applyFont="1" applyBorder="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="8" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="9" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="6" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="13" xfId="6" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="39" fontId="11" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="8" applyFont="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="39" fontId="11" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="39" fontId="11" fillId="0" borderId="14" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="39" fontId="11" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -536,11 +529,7 @@
   <dxfs count="14">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -551,28 +540,52 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF2C5282"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF2C5282"/>
-        </bottom>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
         <vertical style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </vertical>
         <horizontal style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF2C5282"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
         </horizontal>
       </border>
     </dxf>
@@ -601,22 +614,64 @@
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF2C5282"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </bottom>
         <vertical style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </vertical>
         <horizontal style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </horizontal>
       </border>
     </dxf>
@@ -639,19 +694,23 @@
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -669,22 +728,22 @@
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </bottom>
         <vertical style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </vertical>
         <horizontal style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </horizontal>
       </border>
     </dxf>
@@ -704,65 +763,42 @@
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </bottom>
         <vertical style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </vertical>
         <horizontal style="thin">
-          <color rgb="FF2C5282"/>
+          <color indexed="64"/>
         </horizontal>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF2C5282"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF2C5282"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF2C5282"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color rgb="FF2C5282"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF2C5282"/>
-        </horizontal>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF2C5282"/>
+        <left style="thin">
+          <color indexed="64"/>
         </left>
-        <right style="medium">
-          <color rgb="FF2C5282"/>
+        <right style="thin">
+          <color indexed="64"/>
         </right>
-        <top style="medium">
-          <color rgb="FF2C5282"/>
+        <top style="thin">
+          <color indexed="64"/>
         </top>
-        <bottom style="medium">
-          <color rgb="FF2C5282"/>
+        <bottom style="thin">
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -779,45 +815,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF2C5282"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF2C5282"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF2C5282"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF2C5282"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color rgb="FF2C5282"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF2C5282"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -889,26 +886,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TimeSheet" displayName="TimeSheet" ref="A6:E100" headerRowDxfId="9" dataDxfId="7" totalsRowDxfId="5" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A6:E100" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TimeSheet" displayName="TimeSheet" ref="A6:E62" headerRowDxfId="1" dataDxfId="9" totalsRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E62">
-    <sortCondition ref="A7:A100"/>
-    <sortCondition ref="B7:B100"/>
-    <sortCondition ref="C7:C100"/>
-    <sortCondition ref="E7:E100"/>
+    <sortCondition ref="A7:A62"/>
+    <sortCondition ref="B7:B62"/>
+    <sortCondition ref="C7:C62"/>
+    <sortCondition ref="E7:E62"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" totalsRowLabel="Ergebnis" dataDxfId="4" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Project" dataDxfId="3" dataCellStyle="Time"/>
-    <tableColumn id="4" xr3:uid="{5BC75CFE-329B-AC47-8E9D-5F9720844C46}" name="Location" dataDxfId="2" dataCellStyle="Time"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Activity" totalsRowFunction="count" dataDxfId="1" dataCellStyle="Hours"/>
-    <tableColumn id="5" xr3:uid="{61320F46-C251-46E0-8A60-C3960D0324BC}" name="Working Hours" dataDxfId="0" dataCellStyle="Hours"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" totalsRowLabel="Ergebnis" dataDxfId="6" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Project" dataDxfId="5" dataCellStyle="Time"/>
+    <tableColumn id="4" xr3:uid="{5BC75CFE-329B-AC47-8E9D-5F9720844C46}" name="Location" dataDxfId="4" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Activity" totalsRowFunction="count" dataDxfId="3" dataCellStyle="Hours"/>
+    <tableColumn id="5" xr3:uid="{61320F46-C251-46E0-8A60-C3960D0324BC}" name="Working Hours" dataDxfId="2" dataCellStyle="Hours"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1181,10 +1171,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1195,1294 +1185,1028 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="1">
         <v>44562</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="1">
         <v>44926</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="25">
         <v>200</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="10"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
+      <c r="A7" s="6">
         <v>44564</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
+      <c r="A8" s="6">
         <v>44564</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="6">
         <v>44564</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="6">
         <v>44565</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="6">
         <v>44565</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="6">
         <v>44565</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+      <c r="A13" s="6">
         <v>44566</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="6">
         <v>44566</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="6">
         <v>44566</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+      <c r="A16" s="6">
         <v>44567</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+      <c r="A17" s="6">
         <v>44567</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
+      <c r="A18" s="6">
         <v>44567</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+      <c r="A19" s="6">
         <v>44568</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
+      <c r="A20" s="6">
         <v>44568</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+      <c r="A21" s="6">
         <v>44568</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
+      <c r="A22" s="6">
         <v>44571</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="9">
         <v>3.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16">
+      <c r="A23" s="6">
         <v>44571</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="9">
         <v>4.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16">
+      <c r="A24" s="6">
         <v>44572</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="9">
         <v>4.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16">
+      <c r="A25" s="6">
         <v>44572</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="9">
         <v>4.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
+      <c r="A26" s="6">
         <v>44573</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="9">
         <v>5.5</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
+      <c r="A27" s="6">
         <v>44573</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="9">
         <v>4.5</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
+      <c r="A28" s="6">
         <v>44574</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="9">
         <v>6.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
+      <c r="A29" s="6">
         <v>44574</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="9">
         <v>4.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16">
+      <c r="A30" s="6">
         <v>44575</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="9">
         <v>7.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
+      <c r="A31" s="6">
         <v>44575</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="9">
         <v>4.5</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16">
+      <c r="A32" s="6">
         <v>44578</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16">
+      <c r="A33" s="6">
         <v>44578</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C33" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
+      <c r="A34" s="6">
         <v>44578</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16">
+      <c r="A35" s="6">
         <v>44579</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="C35" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16">
+      <c r="A36" s="6">
         <v>44579</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16">
+      <c r="A37" s="6">
         <v>44579</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16">
+      <c r="A38" s="6">
         <v>44580</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="C38" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="16">
+      <c r="A39" s="6">
         <v>44580</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C39" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16">
+      <c r="A40" s="6">
         <v>44580</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16">
+      <c r="A41" s="6">
         <v>44581</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16">
+      <c r="A42" s="6">
         <v>44581</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="16">
+      <c r="A43" s="6">
         <v>44581</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="9">
         <v>9.5</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16">
+      <c r="A44" s="6">
         <v>44582</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C44" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="16">
+      <c r="A45" s="6">
         <v>44582</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="C45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="16">
+      <c r="A46" s="6">
         <v>44582</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="9">
         <v>5.5</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="16">
+      <c r="A47" s="6">
         <v>44585</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="16">
+      <c r="A48" s="6">
         <v>44585</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="16">
+      <c r="A49" s="6">
         <v>44585</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="16">
+      <c r="A50" s="6">
         <v>44586</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C50" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="16">
+      <c r="A51" s="6">
         <v>44586</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="C51" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="16">
+      <c r="A52" s="6">
         <v>44586</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="C52" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E52" s="9">
         <v>9.5</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="16">
+      <c r="A53" s="6">
         <v>44587</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="C53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="17">
+      <c r="E53" s="9">
         <v>0.25</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16">
+      <c r="A54" s="6">
         <v>44587</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="C54" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E54" s="9">
         <v>0.5</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16">
+      <c r="A55" s="6">
         <v>44587</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="C55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E55" s="17">
+      <c r="E55" s="9">
         <v>8.5</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="16">
+      <c r="A56" s="6">
         <v>44588</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="C56" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="9">
         <v>0.25</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="16">
+      <c r="A57" s="6">
         <v>44588</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="C57" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="9">
         <v>0.75</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="16">
+      <c r="A58" s="6">
         <v>44588</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="C58" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="9">
         <v>7.5</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="16">
+      <c r="A59" s="6">
         <v>44589</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="C59" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="17">
+      <c r="E59" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="16">
+      <c r="A60" s="6">
         <v>44589</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="C60" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="9">
         <v>1.75</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="16">
+      <c r="A61" s="6">
         <v>44589</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="C61" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="16">
+      <c r="A62" s="11">
         <v>44592</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="2" t="s">
+      <c r="C62" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="14">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="16"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="16"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="17"/>
-    </row>
-    <row r="65" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="16"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="16"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="17"/>
-    </row>
-    <row r="67" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="16"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="68" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="16"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="16"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="16"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="16"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="17"/>
-    </row>
-    <row r="72" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="16"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="17"/>
-    </row>
-    <row r="73" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="16"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="17"/>
-    </row>
-    <row r="74" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="16"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="17"/>
-    </row>
-    <row r="75" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="16"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="17"/>
-    </row>
-    <row r="76" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="16"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="17"/>
-    </row>
-    <row r="77" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="16"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="17"/>
-    </row>
-    <row r="78" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="16"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="17"/>
-    </row>
-    <row r="79" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="16"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="17"/>
-    </row>
-    <row r="80" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="16"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="17"/>
-    </row>
-    <row r="81" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="16"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="17"/>
-    </row>
-    <row r="82" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="16"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="17"/>
-    </row>
-    <row r="83" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="16"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="17"/>
-    </row>
-    <row r="84" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="16"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="17"/>
-    </row>
-    <row r="85" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="16"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="17"/>
-    </row>
-    <row r="86" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="16"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="17"/>
-    </row>
-    <row r="87" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="16"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="17"/>
-    </row>
-    <row r="88" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="16"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="17"/>
-    </row>
-    <row r="89" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="16"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="17"/>
-    </row>
-    <row r="90" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="16"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="17"/>
-    </row>
-    <row r="91" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="16"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="17"/>
-    </row>
-    <row r="92" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="16"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="17"/>
-    </row>
-    <row r="93" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="16"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="17"/>
-    </row>
-    <row r="94" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="16"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="17"/>
-    </row>
-    <row r="95" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="16"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="17"/>
-    </row>
-    <row r="96" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="16"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="17"/>
-    </row>
-    <row r="97" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="16"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="17"/>
-    </row>
-    <row r="98" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="16"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="17"/>
-    </row>
-    <row r="99" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="16"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="17"/>
-    </row>
-    <row r="100" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19"/>
-      <c r="C100" s="19"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2492,7 +2216,7 @@
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D4:E4 F1:XFD1048576 D6:E1048576 A2:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="D4:E4 A2:C1048576 D6:E1048576 F1:XFD1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="tino@hertlein.dev" xr:uid="{3352D2BA-3859-4F8E-840D-51E5D25E8D16}"/>

</xml_diff>